<commit_message>
gérer les 3 erreurs et autres type d'extract, parsing xl et csv ok  et corriger pdf et alim db
</commit_message>
<xml_diff>
--- a/Downloads/04-01/Source126 - Taux de chômage selon les tranches d'âge au milieu urbain - Trimestriel (10).xlsx
+++ b/Downloads/04-01/Source126 - Taux de chômage selon les tranches d'âge au milieu urbain - Trimestriel (10).xlsx
@@ -690,11 +690,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="156918672"/>
-        <c:axId val="1344820905"/>
+        <c:axId val="1564713245"/>
+        <c:axId val="1546450214"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="156918672"/>
+        <c:axId val="1564713245"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,10 +746,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1344820905"/>
+        <c:crossAx val="1546450214"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1344820905"/>
+        <c:axId val="1546450214"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -825,7 +825,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156918672"/>
+        <c:crossAx val="1564713245"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="5.0"/>
       </c:valAx>

</xml_diff>

<commit_message>
gérer les 3 erreurs et autres type d'extract, parsing xl et csv ok, refactir ok  et corriger pdf et alim db
</commit_message>
<xml_diff>
--- a/Downloads/04-01/Source126 - Taux de chômage selon les tranches d'âge au milieu urbain - Trimestriel (10).xlsx
+++ b/Downloads/04-01/Source126 - Taux de chômage selon les tranches d'âge au milieu urbain - Trimestriel (10).xlsx
@@ -690,11 +690,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1564713245"/>
-        <c:axId val="1546450214"/>
+        <c:axId val="1317466332"/>
+        <c:axId val="564785094"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1564713245"/>
+        <c:axId val="1317466332"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,10 +746,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1546450214"/>
+        <c:crossAx val="564785094"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1546450214"/>
+        <c:axId val="564785094"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -825,7 +825,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1564713245"/>
+        <c:crossAx val="1317466332"/>
         <c:majorUnit val="10.0"/>
         <c:minorUnit val="5.0"/>
       </c:valAx>

</xml_diff>